<commit_message>
added 3 cells at end to get accuracy score for predictions
</commit_message>
<xml_diff>
--- a/ModelTracker.xlsx
+++ b/ModelTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/MIDS/w266/w266_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CBD527-FE3B-0D41-BADA-5A45F38CEE4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE908C7B-F633-F149-BBA5-F9950CE53FC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22580" xr2:uid="{884C85BC-4D65-2F4A-9D76-CC2901CEB1C3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22580" activeTab="1" xr2:uid="{884C85BC-4D65-2F4A-9D76-CC2901CEB1C3}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="6" r:id="rId1"/>
@@ -317,9 +317,6 @@
     <t>remove rows with lengths &gt; 249 and &lt; 20000. Remove punctuation. Lowercase</t>
   </si>
   <si>
-    <t>Fine tune Bert Model to predict. Designed to be run on Google Co-Lan with GPU. Classification layer is  BertForSequenceClassification</t>
-  </si>
-  <si>
     <t>BertForSequenceClassification</t>
   </si>
   <si>
@@ -359,9 +356,6 @@
     <t>RoBERT_Recurrence_over_BERT/train.ipynb</t>
   </si>
   <si>
-    <t>Series of experiments using provided github code based on this paper: https://arxiv.org/abs/1910.10781 (Hierarchical Transformers for Long Document Classification) and https://arxiv.org/abs/1905.05583 (How to Fine-Tune BERT for Text Classification?)</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -387,6 +381,12 @@
   </si>
   <si>
     <t>Encoding done on Bert Base, modelling on Distil Bert</t>
+  </si>
+  <si>
+    <t>Series of experiments using provided github code based on this paper: https://arxiv.org/abs/1910.10781 (Hierarchical Transformers for Long Document Classification) and https://arxiv.org/abs/1905.05583 (How to Fine-Tune BERT for Text Classification?). Code taken from https://github.com/helmy-elrais/RoBERT_Recurrence_over_BERT</t>
+  </si>
+  <si>
+    <t>Fine tune Bert Model to predict. Designed to be run on Google Co-Lan with GPU. Classification layer is  BertForSequenceClassification. Code taken from https://mccormickml.com/2019/07/22/BERT-fine-tuning/</t>
   </si>
 </sst>
 </file>
@@ -500,19 +500,19 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1025,7 +1025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588FE959-A520-D745-8775-C83F040937A8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
@@ -1040,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA47C748-1A41-2345-BD92-6D2443ED4119}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1064,7 +1064,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>8</v>
@@ -1098,10 +1098,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="24">
         <v>44006</v>
       </c>
       <c r="C2" s="23" t="s">
@@ -1110,13 +1110,13 @@
       <c r="D2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="4" t="s">
@@ -1133,13 +1133,13 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21"/>
-      <c r="B3" s="25"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
-      <c r="E3" s="22"/>
+      <c r="E3" s="21"/>
       <c r="F3" s="23"/>
-      <c r="G3" s="22"/>
+      <c r="G3" s="21"/>
       <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
@@ -1154,13 +1154,13 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
-      <c r="B4" s="25"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
-      <c r="E4" s="22"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="23"/>
-      <c r="G4" s="22"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="4" t="s">
         <v>15</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>44013</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>85</v>
@@ -1270,7 +1270,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>90</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>16</v>
@@ -1293,7 +1293,7 @@
         <v>87</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
@@ -1301,33 +1301,33 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="L8" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="24">
+        <v>44002</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="25">
-        <v>44002</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>96</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>43</v>
       </c>
       <c r="F9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="I9" s="18">
         <v>0.7</v>
@@ -1340,23 +1340,23 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="25"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E10" s="23" t="s">
         <v>43</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="I10" s="20"/>
       <c r="J10" s="18"/>
@@ -1365,119 +1365,125 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="24">
         <v>44012</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="21" t="s">
         <v>106</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>108</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>52</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I11" s="1">
         <v>0.57999999999999996</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="34" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="24"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="23"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
       <c r="G12" s="4" t="s">
         <v>52</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I12" s="1">
         <v>0.57999999999999996</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="24"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="23"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
       <c r="G13" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I13" s="15">
         <v>0.65</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="24"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="23"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
       <c r="G14" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I14" s="15">
         <v>0.57999999999999996</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="34" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="24"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="23"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
       <c r="G15" s="4" t="s">
         <v>52</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I15" s="1">
         <v>0.57999999999999996</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="F11:F15"/>
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="B11:B15"/>
     <mergeCell ref="G2:G4"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="C9:C10"/>
@@ -1490,12 +1496,6 @@
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="F2:F4"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="F11:F15"/>
-    <mergeCell ref="E11:E15"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="B11:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>